<commit_message>
Make request start/end inclusive
</commit_message>
<xml_diff>
--- a/data/Sample Requests.xlsx
+++ b/data/Sample Requests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168FFB02-0603-46DB-BD5C-585DE19935BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5D5CC1-D4F8-4396-94F9-47501688AA53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22257" windowHeight="12649" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22257" windowHeight="12649" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bob" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -341,7 +337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -375,7 +371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AEA93F-9436-443D-BFEC-5EF2B77928DB}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -383,10 +379,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>43498</v>
+        <v>43648</v>
       </c>
       <c r="B1" s="1">
-        <v>43499</v>
+        <v>43648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>